<commit_message>
Edited a couple of cheatsheets
</commit_message>
<xml_diff>
--- a/COMP3370 - Computing and the Cloud Cheatsheet.xlsx
+++ b/COMP3370 - Computing and the Cloud Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E5A5E2-0ED9-4AC6-A15E-715B29251D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB128B12-F256-4F01-B725-B2E3B4F65862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-10910" windowWidth="19420" windowHeight="10300" tabRatio="592" firstSheet="9" activeTab="10" xr2:uid="{0D70E819-E99E-4390-80DB-C4E754893F13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="592" activeTab="4" xr2:uid="{0D70E819-E99E-4390-80DB-C4E754893F13}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Systems and Abstraction" sheetId="1" r:id="rId1"/>
@@ -1433,7 +1433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3643,7 +3643,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>447652</xdr:colOff>
+      <xdr:colOff>447653</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>302559</xdr:rowOff>
     </xdr:to>
@@ -5132,14 +5132,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" style="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
     <col min="3" max="16384" width="23.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -5167,7 +5167,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -5178,7 +5178,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="31.5">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -5189,7 +5189,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -5212,11 +5212,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565796D7-D35E-40EB-B305-EFC8618B15BF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" style="1" customWidth="1"/>
@@ -5227,7 +5227,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="120">
       <c r="A2" s="1" t="s">
         <v>221</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="345" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="345">
       <c r="A3" s="1" t="s">
         <v>223</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="285">
       <c r="A4" s="1" t="s">
         <v>228</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="285">
       <c r="A5" s="1" t="s">
         <v>231</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="60">
       <c r="A6" s="1" t="s">
         <v>235</v>
       </c>
@@ -5314,7 +5314,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="75">
       <c r="A7" s="1" t="s">
         <v>237</v>
       </c>
@@ -5335,11 +5335,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE19E9E-A98E-4BE2-B916-3E13EA42D882}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -5350,7 +5350,7 @@
     <col min="7" max="7" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="180">
       <c r="A2" s="1" t="s">
         <v>239</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="90">
       <c r="A3" s="1" t="s">
         <v>243</v>
       </c>
@@ -5418,7 +5418,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
@@ -5430,7 +5430,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5450,7 +5450,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="195">
       <c r="A2" s="1" t="s">
         <v>245</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="285">
       <c r="A3" s="1" t="s">
         <v>250</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="135">
       <c r="A4" s="1" t="s">
         <v>253</v>
       </c>
@@ -5506,7 +5506,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="60.42578125" customWidth="1"/>
@@ -5516,7 +5516,7 @@
     <col min="6" max="6" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -5536,7 +5536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="240">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -5552,7 +5552,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -5564,7 +5564,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="270" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="270">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -5578,7 +5578,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -5590,7 +5590,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="119.25" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -5604,7 +5604,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="105">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -5616,7 +5616,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="90">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -5630,7 +5630,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="105">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -5644,7 +5644,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="135">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -5658,7 +5658,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="165">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
@@ -5672,7 +5672,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="45">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -5686,7 +5686,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="12" t="s">
         <v>45</v>
       </c>
@@ -5711,11 +5711,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7A0F6C-E490-47F6-8F2C-50DF714F8C72}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
@@ -5726,7 +5726,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="75">
       <c r="A2" s="6" t="s">
         <v>47</v>
       </c>
@@ -5758,7 +5758,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="135">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="195">
       <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
@@ -5788,7 +5788,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="270" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="270">
       <c r="A5" s="6" t="s">
         <v>56</v>
       </c>
@@ -5802,7 +5802,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="75">
       <c r="A6" s="6" t="s">
         <v>59</v>
       </c>
@@ -5816,7 +5816,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="120">
       <c r="A7" s="6" t="s">
         <v>62</v>
       </c>
@@ -5830,7 +5830,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="135">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -5861,7 +5861,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
@@ -5871,7 +5871,7 @@
     <col min="6" max="6" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="135">
       <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="90">
       <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
@@ -5925,7 +5925,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="6" t="s">
         <v>76</v>
       </c>
@@ -5941,7 +5941,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>80</v>
       </c>
@@ -5968,21 +5968,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7130233-6AF6-4BA4-B9BA-0FE2F6025445}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
     <col min="4" max="4" width="62.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -6002,7 +6002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="120">
       <c r="A2" s="6" t="s">
         <v>83</v>
       </c>
@@ -6020,7 +6020,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="225">
       <c r="A3" s="6" t="s">
         <v>88</v>
       </c>
@@ -6034,7 +6034,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="90">
       <c r="A4" s="6" t="s">
         <v>91</v>
       </c>
@@ -6046,7 +6046,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="225">
       <c r="A5" s="15" t="s">
         <v>93</v>
       </c>
@@ -6058,7 +6058,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" ht="255" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="255">
       <c r="A6" s="15" t="s">
         <v>95</v>
       </c>
@@ -6070,7 +6070,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="105">
       <c r="A7" s="15" t="s">
         <v>97</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="90">
       <c r="A8" s="15" t="s">
         <v>99</v>
       </c>
@@ -6094,7 +6094,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="120">
       <c r="A9" s="15" t="s">
         <v>101</v>
       </c>
@@ -6125,7 +6125,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
@@ -6135,7 +6135,7 @@
     <col min="6" max="6" width="85.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -6155,7 +6155,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="90">
       <c r="A2" s="6" t="s">
         <v>104</v>
       </c>
@@ -6167,7 +6167,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="330">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -6181,7 +6181,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="150">
       <c r="A4" s="6" t="s">
         <v>109</v>
       </c>
@@ -6199,7 +6199,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="150">
       <c r="A5" s="6" t="s">
         <v>114</v>
       </c>
@@ -6217,7 +6217,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="165">
       <c r="A6" s="6" t="s">
         <v>118</v>
       </c>
@@ -6235,7 +6235,7 @@
       </c>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="240">
       <c r="A7" s="6" t="s">
         <v>122</v>
       </c>
@@ -6251,7 +6251,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="6" t="s">
         <v>126</v>
       </c>
@@ -6263,7 +6263,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="87.75" customHeight="1">
       <c r="A9" s="6" t="s">
         <v>128</v>
       </c>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="104.25" customHeight="1">
       <c r="A10" s="6" t="s">
         <v>131</v>
       </c>
@@ -6291,7 +6291,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="115.5" customHeight="1">
       <c r="A11" s="6" t="s">
         <v>134</v>
       </c>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="96.75" customHeight="1">
       <c r="A12" s="6" t="s">
         <v>137</v>
       </c>
@@ -6319,7 +6319,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="105">
       <c r="A13" s="6" t="s">
         <v>140</v>
       </c>
@@ -6333,7 +6333,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="198" customHeight="1">
       <c r="A14" s="6" t="s">
         <v>143</v>
       </c>
@@ -6343,7 +6343,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="120">
       <c r="A15" s="6" t="s">
         <v>144</v>
       </c>
@@ -6357,7 +6357,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="90">
       <c r="A16" s="6" t="s">
         <v>147</v>
       </c>
@@ -6371,7 +6371,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="45">
       <c r="A17" s="6" t="s">
         <v>150</v>
       </c>
@@ -6383,7 +6383,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="150">
       <c r="A18" s="6" t="s">
         <v>152</v>
       </c>
@@ -6412,7 +6412,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="76" customWidth="1"/>
@@ -6422,7 +6422,7 @@
     <col min="6" max="6" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6442,7 +6442,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="165">
       <c r="A2" s="1" t="s">
         <v>154</v>
       </c>
@@ -6460,7 +6460,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="90">
       <c r="A3" s="1" t="s">
         <v>158</v>
       </c>
@@ -6474,7 +6474,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="90">
       <c r="A4" s="1" t="s">
         <v>161</v>
       </c>
@@ -6486,7 +6486,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>163</v>
       </c>
@@ -6498,7 +6498,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>165</v>
       </c>
@@ -6510,7 +6510,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="1" t="s">
         <v>167</v>
       </c>
@@ -6522,7 +6522,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="1" t="s">
         <v>169</v>
       </c>
@@ -6536,7 +6536,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30">
       <c r="A9" s="1" t="s">
         <v>172</v>
       </c>
@@ -6550,7 +6550,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>175</v>
       </c>
@@ -6562,7 +6562,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30">
       <c r="A11" s="1" t="s">
         <v>177</v>
       </c>
@@ -6574,7 +6574,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="225">
       <c r="A12" s="1" t="s">
         <v>179</v>
       </c>
@@ -6588,7 +6588,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="165">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -6600,7 +6600,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="108.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>184</v>
       </c>
@@ -6612,7 +6612,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="120">
       <c r="A15" s="1" t="s">
         <v>186</v>
       </c>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="240">
       <c r="A16" s="1" t="s">
         <v>191</v>
       </c>
@@ -6659,7 +6659,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
@@ -6669,7 +6669,7 @@
     <col min="6" max="6" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="120">
       <c r="A2" s="1" t="s">
         <v>193</v>
       </c>
@@ -6703,7 +6703,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="210">
       <c r="A3" s="1" t="s">
         <v>196</v>
       </c>
@@ -6721,7 +6721,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="210">
       <c r="A4" s="1" t="s">
         <v>201</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="195">
       <c r="A5" s="1" t="s">
         <v>206</v>
       </c>
@@ -6771,7 +6771,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
@@ -6781,7 +6781,7 @@
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="300" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="300">
       <c r="A2" s="1" t="s">
         <v>210</v>
       </c>
@@ -6817,7 +6817,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="210">
       <c r="A3" s="1" t="s">
         <v>214</v>
       </c>
@@ -6831,7 +6831,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="390" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="390">
       <c r="A4" s="1" t="s">
         <v>217</v>
       </c>
@@ -6858,12 +6858,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6e149233-bc5e-4d60-a409-cb2d210f3947" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7094,17 +7093,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6e149233-bc5e-4d60-a409-cb2d210f3947" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{645C5005-C549-4346-BA2F-9C9A1FB13CB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20058456-57BA-4B0C-8896-BC01F9C02CE3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6e149233-bc5e-4d60-a409-cb2d210f3947"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7129,11 +7131,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20058456-57BA-4B0C-8896-BC01F9C02CE3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{645C5005-C549-4346-BA2F-9C9A1FB13CB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6e149233-bc5e-4d60-a409-cb2d210f3947"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edited HCI cheatsheet slightly
</commit_message>
<xml_diff>
--- a/COMP3370 - Computing and the Cloud Cheatsheet.xlsx
+++ b/COMP3370 - Computing and the Cloud Cheatsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB128B12-F256-4F01-B725-B2E3B4F65862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31E3B81-E01E-41E8-B1B7-54025D3D1C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="592" activeTab="4" xr2:uid="{0D70E819-E99E-4390-80DB-C4E754893F13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="592" firstSheet="2" activeTab="5" xr2:uid="{0D70E819-E99E-4390-80DB-C4E754893F13}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Systems and Abstraction" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="264">
   <si>
     <t>Item</t>
   </si>
@@ -1428,12 +1428,15 @@
     Fault Tolerance and Recovery: The master server plays a crucial role in fault tolerance and recovery mechanisms within GFS. It monitors the health and availability of chunk servers, detects failures, and initiates recovery processes such as chunk migration or replication to maintain data availability and system reliability.
     Metadata Caching: To improve performance and reduce latency, clients may cache metadata obtained from the master server locally. This caching mechanism allows clients to retrieve metadata more quickly for subsequent operations without needing to contact the master server repeatedly.</t>
   </si>
+  <si>
+    <t>Examples: chatbots</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5132,14 +5135,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" style="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
     <col min="3" max="16384" width="23.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5156,7 +5159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -5167,7 +5170,7 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -5178,7 +5181,7 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="31.5">
+    <row r="4" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -5189,7 +5192,7 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
@@ -5216,7 +5219,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" style="1" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" style="1" customWidth="1"/>
@@ -5227,7 +5230,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5247,7 +5250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120">
+    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>221</v>
       </c>
@@ -5255,7 +5258,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="345">
+    <row r="3" spans="1:6" ht="345" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>223</v>
       </c>
@@ -5272,7 +5275,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="285">
+    <row r="4" spans="1:6" ht="285" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>228</v>
       </c>
@@ -5289,7 +5292,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="285">
+    <row r="5" spans="1:6" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>231</v>
       </c>
@@ -5306,7 +5309,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>235</v>
       </c>
@@ -5314,7 +5317,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75">
+    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>237</v>
       </c>
@@ -5339,7 +5342,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
@@ -5350,7 +5353,7 @@
     <col min="7" max="7" width="60.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5370,7 +5373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="180">
+    <row r="2" spans="1:7" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>239</v>
       </c>
@@ -5389,7 +5392,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="90">
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>243</v>
       </c>
@@ -5418,7 +5421,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" style="1" customWidth="1"/>
@@ -5430,7 +5433,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5450,7 +5453,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="195">
+    <row r="2" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>245</v>
       </c>
@@ -5467,7 +5470,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="285">
+    <row r="3" spans="1:6" ht="285" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>250</v>
       </c>
@@ -5481,7 +5484,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="135">
+    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>253</v>
       </c>
@@ -5506,7 +5509,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="60.42578125" customWidth="1"/>
@@ -5516,7 +5519,7 @@
     <col min="6" max="6" width="71.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -5536,7 +5539,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="240">
+    <row r="2" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -5552,7 +5555,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -5564,7 +5567,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="270">
+    <row r="4" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>20</v>
       </c>
@@ -5578,7 +5581,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
@@ -5590,7 +5593,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="119.25" customHeight="1">
+    <row r="6" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -5604,7 +5607,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="105">
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>28</v>
       </c>
@@ -5616,7 +5619,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="1:6" ht="90">
+    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -5630,7 +5633,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="1:6" ht="105">
+    <row r="9" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -5644,7 +5647,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:6" ht="135">
+    <row r="10" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>36</v>
       </c>
@@ -5658,7 +5661,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="1:6" ht="165">
+    <row r="11" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
@@ -5672,7 +5675,7 @@
       </c>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="1:6" ht="45">
+    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -5686,7 +5689,7 @@
       </c>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>45</v>
       </c>
@@ -5715,7 +5718,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
@@ -5726,7 +5729,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5746,7 +5749,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75">
+    <row r="2" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>47</v>
       </c>
@@ -5758,7 +5761,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="135">
+    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
@@ -5774,7 +5777,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="195">
+    <row r="4" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
@@ -5788,7 +5791,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="270">
+    <row r="5" spans="1:6" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>56</v>
       </c>
@@ -5802,7 +5805,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="75">
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>59</v>
       </c>
@@ -5816,7 +5819,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="120">
+    <row r="7" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>62</v>
       </c>
@@ -5830,7 +5833,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="135">
+    <row r="8" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -5861,7 +5864,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
@@ -5871,7 +5874,7 @@
     <col min="6" max="6" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5891,7 +5894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="135">
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
@@ -5907,7 +5910,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="90">
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>72</v>
       </c>
@@ -5925,7 +5928,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>76</v>
       </c>
@@ -5941,7 +5944,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>80</v>
       </c>
@@ -5968,11 +5971,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7130233-6AF6-4BA4-B9BA-0FE2F6025445}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="2" width="57.140625" customWidth="1"/>
@@ -5982,7 +5985,7 @@
     <col min="6" max="6" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -6002,7 +6005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120">
+    <row r="2" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>83</v>
       </c>
@@ -6020,7 +6023,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="225">
+    <row r="3" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>88</v>
       </c>
@@ -6034,7 +6037,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="90">
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>91</v>
       </c>
@@ -6046,7 +6049,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="225">
+    <row r="5" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>93</v>
       </c>
@@ -6058,7 +6061,7 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" ht="255">
+    <row r="6" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>95</v>
       </c>
@@ -6070,7 +6073,7 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" ht="105">
+    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>97</v>
       </c>
@@ -6082,7 +6085,7 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="90">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>99</v>
       </c>
@@ -6094,7 +6097,7 @@
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
     </row>
-    <row r="9" spans="1:6" ht="120">
+    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>101</v>
       </c>
@@ -6121,11 +6124,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7E836C-434F-4798-8C29-1F49AD809155}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
@@ -6135,7 +6138,7 @@
     <col min="6" max="6" width="85.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -6155,7 +6158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="90">
+    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>104</v>
       </c>
@@ -6167,7 +6170,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="330">
+    <row r="3" spans="1:6" ht="330" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>106</v>
       </c>
@@ -6181,7 +6184,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" ht="150">
+    <row r="4" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>109</v>
       </c>
@@ -6199,7 +6202,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="150">
+    <row r="5" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>114</v>
       </c>
@@ -6217,7 +6220,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="165">
+    <row r="6" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>118</v>
       </c>
@@ -6235,7 +6238,7 @@
       </c>
       <c r="F6" s="16"/>
     </row>
-    <row r="7" spans="1:6" ht="240">
+    <row r="7" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>122</v>
       </c>
@@ -6248,10 +6251,12 @@
       <c r="D7" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>263</v>
+      </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>126</v>
       </c>
@@ -6263,7 +6268,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="87.75" customHeight="1">
+    <row r="9" spans="1:6" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>128</v>
       </c>
@@ -6277,7 +6282,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="104.25" customHeight="1">
+    <row r="10" spans="1:6" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>131</v>
       </c>
@@ -6291,7 +6296,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="115.5" customHeight="1">
+    <row r="11" spans="1:6" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>134</v>
       </c>
@@ -6305,7 +6310,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="96.75" customHeight="1">
+    <row r="12" spans="1:6" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>137</v>
       </c>
@@ -6319,7 +6324,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="105">
+    <row r="13" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>140</v>
       </c>
@@ -6333,7 +6338,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" ht="198" customHeight="1">
+    <row r="14" spans="1:6" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>143</v>
       </c>
@@ -6343,7 +6348,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="120">
+    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>144</v>
       </c>
@@ -6357,7 +6362,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="90">
+    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>147</v>
       </c>
@@ -6371,7 +6376,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="45">
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>150</v>
       </c>
@@ -6383,7 +6388,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="150">
+    <row r="18" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>152</v>
       </c>
@@ -6412,7 +6417,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="76" customWidth="1"/>
@@ -6422,7 +6427,7 @@
     <col min="6" max="6" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6442,7 +6447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="165">
+    <row r="2" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>154</v>
       </c>
@@ -6460,7 +6465,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="90">
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>158</v>
       </c>
@@ -6474,7 +6479,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="90">
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>161</v>
       </c>
@@ -6486,7 +6491,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>163</v>
       </c>
@@ -6498,7 +6503,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>165</v>
       </c>
@@ -6510,7 +6515,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="30">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>167</v>
       </c>
@@ -6522,7 +6527,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>169</v>
       </c>
@@ -6536,7 +6541,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="30">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>172</v>
       </c>
@@ -6550,7 +6555,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>175</v>
       </c>
@@ -6562,7 +6567,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="30">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>177</v>
       </c>
@@ -6574,7 +6579,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="225">
+    <row r="12" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>179</v>
       </c>
@@ -6588,7 +6593,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="165">
+    <row r="13" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>182</v>
       </c>
@@ -6600,7 +6605,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" ht="108.75" customHeight="1">
+    <row r="14" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>184</v>
       </c>
@@ -6612,7 +6617,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="120">
+    <row r="15" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>186</v>
       </c>
@@ -6630,7 +6635,7 @@
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="240">
+    <row r="16" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>191</v>
       </c>
@@ -6659,7 +6664,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
@@ -6669,7 +6674,7 @@
     <col min="6" max="6" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6689,7 +6694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="120">
+    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>193</v>
       </c>
@@ -6703,7 +6708,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="210">
+    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>196</v>
       </c>
@@ -6721,7 +6726,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="210">
+    <row r="4" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>201</v>
       </c>
@@ -6738,7 +6743,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="195">
+    <row r="5" spans="1:6" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>206</v>
       </c>
@@ -6771,7 +6776,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
@@ -6781,7 +6786,7 @@
     <col min="6" max="6" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6801,7 +6806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="300">
+    <row r="2" spans="1:6" ht="300" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>210</v>
       </c>
@@ -6817,7 +6822,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="210">
+    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>214</v>
       </c>
@@ -6831,7 +6836,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="390">
+    <row r="4" spans="1:6" ht="390" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>217</v>
       </c>
@@ -6858,11 +6863,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6e149233-bc5e-4d60-a409-cb2d210f3947" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7093,20 +7099,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6e149233-bc5e-4d60-a409-cb2d210f3947" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20058456-57BA-4B0C-8896-BC01F9C02CE3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{645C5005-C549-4346-BA2F-9C9A1FB13CB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="6e149233-bc5e-4d60-a409-cb2d210f3947"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7131,9 +7134,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{645C5005-C549-4346-BA2F-9C9A1FB13CB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20058456-57BA-4B0C-8896-BC01F9C02CE3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="6e149233-bc5e-4d60-a409-cb2d210f3947"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edited + added LlamaIndex cheatsheet
</commit_message>
<xml_diff>
--- a/COMP3370 - Computing and the Cloud Cheatsheet.xlsx
+++ b/COMP3370 - Computing and the Cloud Cheatsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor\My Drive\Cheatsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31E3B81-E01E-41E8-B1B7-54025D3D1C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C8EB38-1CFB-4543-8732-CAD115B130C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="592" firstSheet="2" activeTab="5" xr2:uid="{0D70E819-E99E-4390-80DB-C4E754893F13}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" tabRatio="592" firstSheet="5" activeTab="8" xr2:uid="{0D70E819-E99E-4390-80DB-C4E754893F13}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Systems and Abstraction" sheetId="1" r:id="rId1"/>
@@ -1406,9 +1406,19 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">    Metadata Management: The master server maintains metadata, which includes information such as file-to-chunk mappings, locations of replicas, and other essential details about the file system. When a client needs to read or write data, it first contacts the master server to obtain metadata related to the operation.
+    Chunk Location Lookup: Upon receiving a request from a client, the master server provides the client with the locations (IP addresses) of the chunk servers storing the relevant data chunks for the requested file. The client then communicates directly with these chunk servers to access the data.
+    Coordination and Control: The master server coordinates various operations within the GFS cluster, such as file creation, deletion, and replication. It ensures data consistency and integrity by managing the placement and replication of data chunks across chunk servers.
+    Fault Tolerance and Recovery: The master server plays a crucial role in fault tolerance and recovery mechanisms within GFS. It monitors the health and availability of chunk servers, detects failures, and initiates recovery processes such as chunk migration or replication to maintain data availability and system reliability.
+    Metadata Caching: To improve performance and reduce latency, clients may cache metadata obtained from the master server locally. This caching mechanism allows clients to retrieve metadata more quickly for subsequent operations without needing to contact the master server repeatedly.</t>
+  </si>
+  <si>
+    <t>Examples: chatbots</t>
+  </si>
+  <si>
     <t>Example of how the data changes from stage to stage:
 pages = [(1, "abc"), (2, "bcd"), (3, "acdef")]
-map stage::
+map stage:
 [(1, a), (1, b), (1, c),
 (2, b), (2, c), (2, d),
 (3, a), (3, c), (3, d), (3, e), (3, f)]
@@ -1420,16 +1430,6 @@
 e: [3],
 f: [3]
 ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Metadata Management: The master server maintains metadata, which includes information such as file-to-chunk mappings, locations of replicas, and other essential details about the file system. When a client needs to read or write data, it first contacts the master server to obtain metadata related to the operation.
-    Chunk Location Lookup: Upon receiving a request from a client, the master server provides the client with the locations (IP addresses) of the chunk servers storing the relevant data chunks for the requested file. The client then communicates directly with these chunk servers to access the data.
-    Coordination and Control: The master server coordinates various operations within the GFS cluster, such as file creation, deletion, and replication. It ensures data consistency and integrity by managing the placement and replication of data chunks across chunk servers.
-    Fault Tolerance and Recovery: The master server plays a crucial role in fault tolerance and recovery mechanisms within GFS. It monitors the health and availability of chunk servers, detects failures, and initiates recovery processes such as chunk migration or replication to maintain data availability and system reliability.
-    Metadata Caching: To improve performance and reduce latency, clients may cache metadata obtained from the master server locally. This caching mechanism allows clients to retrieve metadata more quickly for subsequent operations without needing to contact the master server repeatedly.</t>
-  </si>
-  <si>
-    <t>Examples: chatbots</t>
   </si>
 </sst>
 </file>
@@ -4367,7 +4367,7 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>493057</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2644588</xdr:rowOff>
+      <xdr:rowOff>2473138</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5215,8 +5215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{565796D7-D35E-40EB-B305-EFC8618B15BF}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A5" zoomScale="121" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5286,7 +5286,7 @@
         <v>229</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>230</v>
@@ -5303,7 +5303,7 @@
         <v>233</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>234</v>
@@ -5338,8 +5338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EE19E9E-A98E-4BE2-B916-3E13EA42D882}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="113" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5417,8 +5417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378791C9-6AAD-496A-BABA-0F79C9FED179}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="D3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A2" zoomScale="103" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5478,7 +5478,7 @@
         <v>251</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>252</v>
@@ -6124,8 +6124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7E836C-434F-4798-8C29-1F49AD809155}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6252,7 +6252,7 @@
         <v>125</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F7" s="6"/>
     </row>
@@ -6413,8 +6413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC361287-B3FA-4754-8F77-810CB15EE32E}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6660,8 +6660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C69C5C4-3650-49F2-8C93-570D3130646B}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6772,7 +6772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B336B275-13AB-4CD2-BE95-FCA1A58FF0F9}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>